<commit_message>
Add read boolean column
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="780" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -454,6 +454,16 @@
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>